<commit_message>
#44360 EPPlus can not calculate with Ranges - IF-Function
</commit_message>
<xml_diff>
--- a/EPPlusTest/Resources/Issue_WithRangeCalculation.xlsx
+++ b/EPPlusTest/Resources/Issue_WithRangeCalculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projekte\EPPlus\EPPlus010818\EPPlusTest\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D599FC29-2092-47BB-86D2-02FDE63A6075}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{30DA129A-D3E4-4881-B4DA-69FEA99A6128}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,10 +16,17 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="IB_Q1_AJ">Tabelle1!$C$2:$C$5</definedName>
+    <definedName name="IB_Q2_AJ">Tabelle1!$B$2:$B$5</definedName>
+    <definedName name="IB_Q3_AJ">Tabelle1!$B$2:$B$5</definedName>
     <definedName name="range1">Tabelle1!$A$1:$A$15</definedName>
     <definedName name="range2">Tabelle1!$B$1:$B$15</definedName>
     <definedName name="range3">Tabelle1!$F$19:$R$19</definedName>
     <definedName name="range4">Tabelle1!$F$20:$R$20</definedName>
+    <definedName name="sn_duedate">Tabelle1!$E$2</definedName>
+    <definedName name="sn_duedate1">Tabelle1!$E$3</definedName>
+    <definedName name="sn_duedate2">Tabelle1!$E$4</definedName>
+    <definedName name="sn_duedate3">Tabelle1!$E$5</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -31,9 +38,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>string</t>
+  </si>
+  <si>
+    <t>31.3.</t>
+  </si>
+  <si>
+    <t>30.6.</t>
+  </si>
+  <si>
+    <t>30.9.</t>
+  </si>
+  <si>
+    <t>20.1.</t>
   </si>
 </sst>
 </file>
@@ -69,8 +88,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -385,18 +405,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>I20+1+O21</f>
         <v>211</v>
@@ -405,11 +426,27 @@
         <v>100</v>
       </c>
       <c r="C1">
-        <f t="shared" ref="C1:C15" si="0">range1 + range2</f>
+        <f t="shared" ref="C1:C16" si="0">range1 + range2</f>
         <v>311</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H1" t="e">
+        <f t="shared" ref="H1:H6" si="1">IF(sn_duedate="31.3.",IB_Q1_AJ,IF(sn_duedate="30.6.",IB_Q2_AJ,IF(sn_duedate="30.9.",IB_Q3_AJ,"Falsche Auswahl")))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I1" t="e">
+        <f t="shared" ref="I1:I6" si="2">IF(sn_duedate1="31.3.",IB_Q1_AJ,IF(sn_duedate1="30.6.",IB_Q2_AJ,IF(sn_duedate1="30.9.",IB_Q3_AJ,"Falsche Auswahl")))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J1" t="e">
+        <f t="shared" ref="J1:J6" si="3">IF(sn_duedate2="31.3.",IB_Q1_AJ,IF(sn_duedate2="30.6.",IB_Q2_AJ,IF(sn_duedate2="30.9.",IB_Q3_AJ,"Falsche Auswahl")))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K1" t="str">
+        <f t="shared" ref="K1:K6" si="4">IF(sn_duedate3="31.3.",IB_Q1_AJ,IF(sn_duedate3="30.6.",IB_Q2_AJ,IF(sn_duedate3="30.9.",IB_Q3_AJ,"Falsche Auswahl")))</f>
+        <v>Falsche Auswahl</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>G21+I19+range2</f>
         <v>206</v>
@@ -421,8 +458,27 @@
         <f t="shared" si="0"/>
         <v>306</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <f t="shared" si="1"/>
+        <v>306</v>
+      </c>
+      <c r="I2">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="J2">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="K2" t="str">
+        <f t="shared" si="4"/>
+        <v>Falsche Auswahl</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -433,8 +489,27 @@
         <f t="shared" si="0"/>
         <v>103</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="1"/>
+        <v>103</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" si="4"/>
+        <v>Falsche Auswahl</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -445,8 +520,27 @@
         <f t="shared" si="0"/>
         <v>104</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="4"/>
+        <v>Falsche Auswahl</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -457,8 +551,27 @@
         <f t="shared" si="0"/>
         <v>105</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="4"/>
+        <v>Falsche Auswahl</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -469,8 +582,24 @@
         <f t="shared" si="0"/>
         <v>106</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H6" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I6" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J6" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="4"/>
+        <v>Falsche Auswahl</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -482,7 +611,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -494,7 +623,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -506,7 +635,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -518,7 +647,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>100</v>
       </c>
@@ -526,8 +655,12 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <f>IF(0=1,1,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
@@ -538,8 +671,12 @@
         <f t="shared" si="0"/>
         <v>112</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <f>IF(0=0,1,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
@@ -551,7 +688,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
@@ -563,7 +700,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -575,7 +712,19 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>20</v>
+      </c>
+      <c r="C16" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>99</v>
       </c>
@@ -587,7 +736,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -638,7 +787,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>20</v>
       </c>
@@ -686,61 +835,70 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E21" t="e">
+        <f t="shared" ref="E21:S21" si="5">range3+range4</f>
+        <v>#VALUE!</v>
+      </c>
       <c r="F21">
-        <f t="shared" ref="F21:R21" si="1">range3+range4</f>
+        <f t="shared" si="5"/>
         <v>101</v>
       </c>
       <c r="G21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>102</v>
       </c>
       <c r="H21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>103</v>
       </c>
       <c r="I21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
       <c r="J21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>105</v>
       </c>
       <c r="K21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>106</v>
       </c>
       <c r="L21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>107</v>
       </c>
       <c r="M21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>108</v>
       </c>
       <c r="N21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>109</v>
       </c>
       <c r="O21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>110</v>
       </c>
       <c r="P21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>111</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>112</v>
       </c>
       <c r="R21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>113</v>
+      </c>
+      <c r="S21" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#44360 EPPlus can not calculate with Ranges - single Range in Formula
</commit_message>
<xml_diff>
--- a/EPPlusTest/Resources/Issue_WithRangeCalculation.xlsx
+++ b/EPPlusTest/Resources/Issue_WithRangeCalculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projekte\EPPlus\EPPlus010818\EPPlusTest\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{30DA129A-D3E4-4881-B4DA-69FEA99A6128}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C997DD21-A2AE-413D-994B-09F7EC7E247F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,9 +16,11 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="AGAIN">Tabelle1!$A$2:$A$5</definedName>
     <definedName name="IB_Q1_AJ">Tabelle1!$C$2:$C$5</definedName>
     <definedName name="IB_Q2_AJ">Tabelle1!$B$2:$B$5</definedName>
     <definedName name="IB_Q3_AJ">Tabelle1!$B$2:$B$5</definedName>
+    <definedName name="IF_AGAIN">Tabelle1!$H$2:$H$6</definedName>
     <definedName name="range1">Tabelle1!$A$1:$A$15</definedName>
     <definedName name="range2">Tabelle1!$B$1:$B$15</definedName>
     <definedName name="range3">Tabelle1!$F$19:$R$19</definedName>
@@ -408,7 +410,7 @@
   <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,7 +419,7 @@
     <col min="11" max="11" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>I20+1+O21</f>
         <v>211</v>
@@ -446,7 +448,7 @@
         <v>Falsche Auswahl</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>G21+I19+range2</f>
         <v>206</v>
@@ -461,6 +463,10 @@
       <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="F2">
+        <f>AGAIN</f>
+        <v>206</v>
+      </c>
       <c r="H2">
         <f t="shared" si="1"/>
         <v>306</v>
@@ -477,8 +483,12 @@
         <f t="shared" si="4"/>
         <v>Falsche Auswahl</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <f t="shared" ref="M1:M6" si="5">IF_AGAIN</f>
+        <v>306</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -491,6 +501,10 @@
       </c>
       <c r="E3" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="F3">
+        <f>AGAIN</f>
+        <v>3</v>
       </c>
       <c r="H3">
         <f t="shared" si="1"/>
@@ -508,8 +522,12 @@
         <f t="shared" si="4"/>
         <v>Falsche Auswahl</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <f t="shared" si="5"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -522,6 +540,10 @@
       </c>
       <c r="E4" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="F4">
+        <f>AGAIN</f>
+        <v>4</v>
       </c>
       <c r="H4">
         <f t="shared" si="1"/>
@@ -539,8 +561,12 @@
         <f t="shared" si="4"/>
         <v>Falsche Auswahl</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <f t="shared" si="5"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -553,6 +579,10 @@
       </c>
       <c r="E5" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F5">
+        <f>AGAIN</f>
+        <v>5</v>
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
@@ -570,8 +600,12 @@
         <f t="shared" si="4"/>
         <v>Falsche Auswahl</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <f t="shared" si="5"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -598,8 +632,12 @@
         <f t="shared" si="4"/>
         <v>Falsche Auswahl</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M6" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -611,7 +649,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -623,7 +661,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -635,7 +673,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -647,7 +685,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>100</v>
       </c>
@@ -660,7 +698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
@@ -676,7 +714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
@@ -688,7 +726,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
@@ -700,7 +738,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -712,7 +750,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -837,63 +875,63 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E21" t="e">
-        <f t="shared" ref="E21:S21" si="5">range3+range4</f>
+        <f t="shared" ref="E21:S21" si="6">range3+range4</f>
         <v>#VALUE!</v>
       </c>
       <c r="F21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>101</v>
       </c>
       <c r="G21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>102</v>
       </c>
       <c r="H21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>103</v>
       </c>
       <c r="I21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>104</v>
       </c>
       <c r="J21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>105</v>
       </c>
       <c r="K21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>106</v>
       </c>
       <c r="L21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>107</v>
       </c>
       <c r="M21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>108</v>
       </c>
       <c r="N21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>109</v>
       </c>
       <c r="O21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>110</v>
       </c>
       <c r="P21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>111</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>112</v>
       </c>
       <c r="R21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>113</v>
       </c>
       <c r="S21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
     </row>

</xml_diff>